<commit_message>
Auto-committed on 2022/11/09 週三 12:04:52.99
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/ClFac.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/ClFac.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38570275-8FDD-44B0-8278-83D62623D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D038797-8A19-4BA9-BC38-3B343AE17F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1452" windowWidth="18780" windowHeight="11508" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -464,6 +474,10 @@
   </si>
   <si>
     <t>clMainFirst</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>selecrFroL2411</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1953,9 +1967,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
@@ -2119,6 +2133,14 @@
         <v>93</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/02/17 週五 17:18:19.26
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/ClFac.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/ClFac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L2-業務作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D038797-8A19-4BA9-BC38-3B343AE17F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEFC970-374A-4D19-94B1-D9CB6D5A2A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -409,9 +409,6 @@
   <si>
     <t xml:space="preserve">CustNo = ,AND FacmNo =  ,AND MainFlag = </t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>規劃調整為ApplNo</t>
   </si>
   <si>
     <t>OriSettingAmt</t>
@@ -655,11 +652,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -668,9 +665,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -680,16 +674,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,9 +692,6 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -711,9 +702,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1067,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="72.88671875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1076,875 +1064,873 @@
     <col min="1" max="1" width="5.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.5546875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="72.88671875" style="4"/>
+    <col min="8" max="16384" width="72.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>1</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="D12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>2</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="16">
+        <v>2</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="16">
+        <v>7</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
         <v>4</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="B15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="16">
+        <v>7</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
         <v>5</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="B16" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="16">
+        <v>7</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
         <v>6</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="B17" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="16">
+        <v>3</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
         <v>7</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="B18" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
         <v>8</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="B19" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
-        <v>1</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="B20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
+      <c r="E20" s="16">
+        <v>16</v>
+      </c>
+      <c r="F20" s="16">
         <v>2</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="18" t="s">
+      <c r="G20" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>10</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E21" s="17">
+        <v>16</v>
+      </c>
+      <c r="F21" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
+      <c r="G21" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>11</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>12</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="18">
-        <v>7</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
-        <v>4</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="18">
-        <v>7</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
-        <v>5</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="18">
-        <v>7</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="E23" s="16">
         <v>6</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>13</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>14</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
-        <v>7</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>8</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="20">
-        <v>1</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
-        <v>9</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="18">
-        <v>16</v>
-      </c>
-      <c r="F20" s="18">
-        <v>2</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
-        <v>10</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="20">
-        <v>16</v>
-      </c>
-      <c r="F21" s="20">
-        <v>2</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
-        <v>11</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
-        <v>12</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="E25" s="16">
         <v>6</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="18">
-        <v>13</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
-        <v>14</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="18">
-        <v>6</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1969,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
@@ -1983,13 +1969,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2001,7 +1987,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2012,7 +1998,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2023,7 +2009,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2034,7 +2020,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2045,7 +2031,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2056,40 +2042,40 @@
         <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2100,7 +2086,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2111,31 +2097,31 @@
         <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>53</v>

</xml_diff>